<commit_message>
Charts added to project report part a
</commit_message>
<xml_diff>
--- a/CSV/partA/MasterPartA.xlsx
+++ b/CSV/partA/MasterPartA.xlsx
@@ -1,42 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejayb\HealthDataAnalytics\Iowa_Proj1\CSV\partA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camireittinger/Documents/GitHub/Iowa_Proj1/CSV/partA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBD5F30-B20F-438D-BACC-8B62C0134821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE77A661-F7E6-554C-9CB8-F478E84EBF45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$69</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$70:$A$154</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$69</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$70:$A$154</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$69</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$70:$B$154</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$69</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$70:$C$154</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$D$69</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$70:$D$154</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$E$69</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$E$70:$E$154</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$69</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$70:$B$154</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$69</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$70:$C$154</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$69</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$70:$D$154</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$69</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$70:$E$154</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -340,6 +318,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -355,6 +338,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -370,6 +358,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -385,6 +378,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -400,6 +398,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -415,6 +418,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -432,6 +440,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -449,6 +462,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -466,6 +484,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -483,6 +506,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -500,6 +528,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-240C-834C-BCBF-9E0EFA7D738A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -858,6 +891,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -873,6 +911,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -890,6 +933,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -907,6 +955,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -924,6 +977,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -941,6 +999,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -958,6 +1021,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -975,6 +1043,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-37BF-7A43-BF26-534997248473}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2307,7 +2380,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>COVID Phase Date</a:t>
+              <a:t>COVID Phase Data</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2640,10 +2713,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.0085425642549396E-2"/>
-          <c:y val="0.70074616608086082"/>
+          <c:x val="4.4117670052721859E-3"/>
+          <c:y val="0.77169039367242831"/>
           <c:w val="0.97668449462685103"/>
-          <c:h val="0.27431617805879005"/>
+          <c:h val="0.22804703313106436"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2754,13 +2827,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hepatitis A, Covid </a:t>
+              <a:t>Phase</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Phase Date</a:t>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Data</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2806,7 +2877,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Hepatitis Phase Date</c:v>
+            <c:v>Hepatitis Phase Data</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2901,7 +2972,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Covid Phase Date</c:v>
+            <c:v>Covid Phase Data</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -3284,7 +3355,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hepatitis A Phase Date</a:t>
+              <a:t>Hepatitis A Phase Data</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3618,9 +3689,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="1.0085425642549396E-2"/>
-          <c:y val="0.70074616608086082"/>
+          <c:y val="0.76097752994556567"/>
           <c:w val="0.97668449462685103"/>
-          <c:h val="0.27431617805879005"/>
+          <c:h val="0.2140845706965315"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3990,15 +4061,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hepatitis A, Covid </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
               <a:t>Result Availability</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4006,8 +4070,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.24753799835396459"/>
-          <c:y val="4.6013622125507289E-2"/>
+          <c:x val="0.35786047945000066"/>
+          <c:y val="2.3504711292853062E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4832,6 +4896,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-921A-AE48-A69F-973FD2019F66}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4899,8 +4968,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.0085425642549396E-2"/>
-          <c:y val="0.70074616608086082"/>
+          <c:x val="3.5491763535426789E-3"/>
+          <c:y val="0.72383257384555322"/>
           <c:w val="0.97668449462685103"/>
           <c:h val="0.27431617805879005"/>
         </c:manualLayout>
@@ -5237,13 +5306,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hepatitis A, Covid </a:t>
+              <a:t>Type</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Study Type</a:t>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Trial</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -5253,8 +5320,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.24753799835396459"/>
-          <c:y val="4.6013622125507289E-2"/>
+          <c:x val="0.41346727948282896"/>
+          <c:y val="1.9760449127739225E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -6032,15 +6099,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$69</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Covid 19 Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Months</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -6574,7 +6633,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hepatitis Study Duration</a:t>
+              <a:t>Hepatitis A Study Duration</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6618,15 +6677,7 @@
           <c:idx val="4"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$69</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hepatitis A Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Months</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -12073,6 +12124,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -12089,6 +12145,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -12105,6 +12166,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -12121,6 +12187,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -12137,6 +12208,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -12153,6 +12229,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -12169,6 +12250,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -12185,6 +12271,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -12201,6 +12292,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -12217,6 +12313,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -12233,6 +12334,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-976E-EE48-873B-A0C9984FF59F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -12380,6 +12486,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="552936352"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -12493,6 +12600,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="552940944"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -12613,7 +12721,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hepatitis A, Covid Activity Status</a:t>
+              <a:t>Activity Status</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -13156,6 +13264,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-07F4-D34E-9F6F-63B6583BCB71}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -13171,6 +13284,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-07F4-D34E-9F6F-63B6583BCB71}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -13462,6 +13580,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-E533-2041-8596-2217A9C00863}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -13477,6 +13600,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-E533-2041-8596-2217A9C00863}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -13653,10 +13781,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Hepatitis A, Covid </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
@@ -13706,7 +13830,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Hepatitis Activity Status</c:v>
+            <c:v>Hepatitis Gender</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -13771,7 +13895,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Covid Activity Status</c:v>
+            <c:v>Covid Gender</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -30478,16 +30602,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>1691640</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>438854</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>506307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>522675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>790223</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30631,15 +30755,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
+      <xdr:colOff>236219</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>701040</xdr:rowOff>
+      <xdr:rowOff>701039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>620888</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30707,15 +30831,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:colOff>601979</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>662940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>395110</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>56444</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30785,13 +30909,13 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>295038</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>30479</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>388619</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>1965887</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>56445</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30896,16 +31020,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>607458</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141792</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>22859</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>91439</xdr:colOff>
-      <xdr:row>168</xdr:row>
-      <xdr:rowOff>129467</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>451556</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>98778</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -30973,13 +31097,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
+      <xdr:colOff>68579</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>169332</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
@@ -31009,13 +31133,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
+      <xdr:colOff>68579</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>169332</xdr:colOff>
       <xdr:row>98</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
@@ -31540,23 +31664,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AJ159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -31573,7 +31697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -31595,7 +31719,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -31614,7 +31738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -31633,7 +31757,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -31652,7 +31776,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -31671,7 +31795,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -31690,7 +31814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -31709,7 +31833,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -31728,7 +31852,7 @@
         <v>5.6338028169014086E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -31747,7 +31871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -31766,7 +31890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -31785,8 +31909,8 @@
         <v>8.4507042253521125E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="50.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="50.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -31803,7 +31927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -31824,7 +31948,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -31845,8 +31969,8 @@
         <v>0.98591549295774639</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="138.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="138.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -31860,7 +31984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -31879,7 +32003,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -31898,7 +32022,7 @@
         <v>0.9859154929577465</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -31917,7 +32041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -31936,8 +32060,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="85.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -31954,7 +32078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0</v>
       </c>
@@ -31973,7 +32097,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -31992,7 +32116,7 @@
         <v>0.39436619718309857</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -32011,7 +32135,7 @@
         <v>0.26760563380281688</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -32030,7 +32154,7 @@
         <v>0.15492957746478872</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -32049,7 +32173,7 @@
         <v>8.4507042253521125E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>5</v>
       </c>
@@ -32068,7 +32192,7 @@
         <v>5.6338028169014086E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>6</v>
       </c>
@@ -32087,7 +32211,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>7</v>
       </c>
@@ -32106,7 +32230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8</v>
       </c>
@@ -32125,7 +32249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>11</v>
       </c>
@@ -32144,7 +32268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>12</v>
       </c>
@@ -32163,7 +32287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>16</v>
       </c>
@@ -32182,7 +32306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>30</v>
       </c>
@@ -32201,8 +32325,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="264.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -32219,7 +32343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -32238,7 +32362,7 @@
         <v>1.3245033112582781E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -32257,7 +32381,7 @@
         <v>3.3112582781456956E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -32276,7 +32400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -32295,7 +32419,7 @@
         <v>6.6225165562913907E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -32314,7 +32438,7 @@
         <v>2.6490066225165563E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -32333,7 +32457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -32352,7 +32476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -32371,7 +32495,7 @@
         <v>2.6490066225165563E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -32390,7 +32514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -32409,7 +32533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -32428,7 +32552,7 @@
         <v>0.85430463576158944</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -32447,8 +32571,8 @@
         <v>3.9735099337748346E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="56.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -32465,7 +32589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -32484,7 +32608,7 @@
         <v>0.11267605633802817</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -32503,7 +32627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -32522,7 +32646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -32541,7 +32665,7 @@
         <v>7.0422535211267609E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -32560,7 +32684,7 @@
         <v>0.26760563380281688</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>38</v>
       </c>
@@ -32579,7 +32703,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>39</v>
       </c>
@@ -32598,7 +32722,7 @@
         <v>0.45070422535211269</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>40</v>
       </c>
@@ -32617,7 +32741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -32636,8 +32760,8 @@
         <v>7.0422535211267609E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="103.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="103.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>53</v>
       </c>
@@ -32654,7 +32778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -32673,7 +32797,7 @@
         <v>0.36619718309859156</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -32692,8 +32816,8 @@
         <v>0.63380281690140849</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="162" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="162" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -32710,7 +32834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>0</v>
       </c>
@@ -32729,7 +32853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1</v>
       </c>
@@ -32748,7 +32872,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
@@ -32767,7 +32891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>3</v>
       </c>
@@ -32786,7 +32910,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>4</v>
       </c>
@@ -32805,7 +32929,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>5</v>
       </c>
@@ -32824,7 +32948,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>6</v>
       </c>
@@ -32843,7 +32967,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>7</v>
       </c>
@@ -32862,7 +32986,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>8</v>
       </c>
@@ -32881,7 +33005,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>9</v>
       </c>
@@ -32900,7 +33024,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>10</v>
       </c>
@@ -32919,7 +33043,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>11</v>
       </c>
@@ -32938,7 +33062,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>12</v>
       </c>
@@ -32957,7 +33081,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>13</v>
       </c>
@@ -32976,7 +33100,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>14</v>
       </c>
@@ -32995,7 +33119,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>15</v>
       </c>
@@ -33014,7 +33138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>16</v>
       </c>
@@ -33033,7 +33157,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>17</v>
       </c>
@@ -33052,7 +33176,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>18</v>
       </c>
@@ -33071,7 +33195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>19</v>
       </c>
@@ -33090,7 +33214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>20</v>
       </c>
@@ -33109,7 +33233,7 @@
         <v>5.7971014492753624E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>21</v>
       </c>
@@ -33128,7 +33252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>22</v>
       </c>
@@ -33147,7 +33271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>23</v>
       </c>
@@ -33166,7 +33290,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>24</v>
       </c>
@@ -33185,7 +33309,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>25</v>
       </c>
@@ -33204,7 +33328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>26</v>
       </c>
@@ -33223,7 +33347,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>27</v>
       </c>
@@ -33242,7 +33366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>28</v>
       </c>
@@ -33261,7 +33385,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>29</v>
       </c>
@@ -33280,7 +33404,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>30</v>
       </c>
@@ -33299,7 +33423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>31</v>
       </c>
@@ -33318,7 +33442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>32</v>
       </c>
@@ -33337,7 +33461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>33</v>
       </c>
@@ -33356,7 +33480,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>34</v>
       </c>
@@ -33375,7 +33499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>35</v>
       </c>
@@ -33394,7 +33518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>36</v>
       </c>
@@ -33413,7 +33537,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>37</v>
       </c>
@@ -33432,7 +33556,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>38</v>
       </c>
@@ -33451,7 +33575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>39</v>
       </c>
@@ -33470,7 +33594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>40</v>
       </c>
@@ -33489,7 +33613,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>42</v>
       </c>
@@ -33508,7 +33632,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>43</v>
       </c>
@@ -33527,7 +33651,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>46</v>
       </c>
@@ -33546,7 +33670,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>47</v>
       </c>
@@ -33565,7 +33689,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>48</v>
       </c>
@@ -33584,7 +33708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>49</v>
       </c>
@@ -33603,7 +33727,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>50</v>
       </c>
@@ -33622,7 +33746,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>264</v>
       </c>
@@ -33641,7 +33765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>128</v>
       </c>
@@ -33660,7 +33784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>52</v>
       </c>
@@ -33679,7 +33803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>53</v>
       </c>
@@ -33698,7 +33822,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>54</v>
       </c>
@@ -33717,7 +33841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>56</v>
       </c>
@@ -33736,7 +33860,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>57</v>
       </c>
@@ -33755,7 +33879,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>58</v>
       </c>
@@ -33774,7 +33898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>59</v>
       </c>
@@ -33793,7 +33917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>60</v>
       </c>
@@ -33812,7 +33936,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>138</v>
       </c>
@@ -33831,7 +33955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>62</v>
       </c>
@@ -33850,7 +33974,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>63</v>
       </c>
@@ -33869,7 +33993,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>65</v>
       </c>
@@ -33888,7 +34012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>67</v>
       </c>
@@ -33907,7 +34031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>68</v>
       </c>
@@ -33926,7 +34050,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>69</v>
       </c>
@@ -33945,7 +34069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>72</v>
       </c>
@@ -33964,7 +34088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>129</v>
       </c>
@@ -33983,7 +34107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>74</v>
       </c>
@@ -34002,7 +34126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>76</v>
       </c>
@@ -34021,7 +34145,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>78</v>
       </c>
@@ -34040,7 +34164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>207</v>
       </c>
@@ -34059,7 +34183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>49</v>
       </c>
@@ -34078,7 +34202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>84</v>
       </c>
@@ -34097,7 +34221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>86</v>
       </c>
@@ -34116,7 +34240,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>90</v>
       </c>
@@ -34135,7 +34259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>92</v>
       </c>
@@ -34154,7 +34278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>94</v>
       </c>
@@ -34173,7 +34297,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>956</v>
       </c>
@@ -34192,7 +34316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>110</v>
       </c>
@@ -34211,7 +34335,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>239</v>
       </c>
@@ -34230,7 +34354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>114</v>
       </c>
@@ -34249,7 +34373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>118</v>
       </c>
@@ -34268,7 +34392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>120</v>
       </c>
@@ -34287,7 +34411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>121</v>
       </c>
@@ -34306,7 +34430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>123</v>
       </c>
@@ -34325,7 +34449,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>49</v>
       </c>
@@ -34342,7 +34466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>46</v>
       </c>
@@ -34361,7 +34485,7 @@
         <v>0.11267605633802817</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>47</v>
       </c>
@@ -34380,7 +34504,7 @@
         <v>0.88732394366197187</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
part c in progress
</commit_message>
<xml_diff>
--- a/CSV/partA/MasterPartA.xlsx
+++ b/CSV/partA/MasterPartA.xlsx
@@ -1,42 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejayb\HealthDataAnalytics\Iowa_Proj1\CSV\partA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\choij\OneDrive\바탕 화면\SP2021\UOI\proj1\CSV\partA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBD5F30-B20F-438D-BACC-8B62C0134821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCE78AE-7EF4-4224-853A-0A6E94D76293}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$69</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$70:$A$154</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$69</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$70:$A$154</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$69</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$70:$B$154</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$69</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$70:$C$154</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$D$69</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$70:$D$154</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$E$69</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$E$70:$E$154</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$69</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$70:$B$154</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$69</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$70:$C$154</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$69</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$70:$D$154</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$69</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$70:$E$154</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -340,6 +318,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -355,6 +338,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -370,6 +358,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -385,6 +378,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -400,6 +398,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -415,6 +418,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -432,6 +440,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -449,6 +462,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -466,6 +484,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -483,6 +506,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -500,6 +528,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-3FC1-4E57-8709-D3BBAAC41380}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -858,6 +891,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -873,6 +911,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -890,6 +933,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -907,6 +955,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -924,6 +977,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -941,6 +999,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -958,6 +1021,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -975,6 +1043,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-6198-406F-B3B4-8F4BCA69E104}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4832,6 +4905,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6C5B-4DF2-9304-6638735A1094}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -12073,6 +12151,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -12089,6 +12172,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -12105,6 +12193,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -12121,6 +12214,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -12137,6 +12235,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -12153,6 +12256,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -12169,6 +12277,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -12185,6 +12298,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -12201,6 +12319,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -12217,6 +12340,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -12233,6 +12361,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-7B72-40DD-95EF-62404D5E6952}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -12380,6 +12513,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="552936352"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -12493,6 +12627,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="552940944"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -13156,6 +13291,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B889-4EF9-B244-A1534940447D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -13171,6 +13311,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B889-4EF9-B244-A1534940447D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -13462,6 +13607,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8B04-4BCA-84E6-C7686AB23CF7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -13477,6 +13627,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8B04-4BCA-84E6-C7686AB23CF7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -31540,23 +31695,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AJ159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B119" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -31573,7 +31728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -31595,7 +31750,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -31614,7 +31769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -31633,7 +31788,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -31652,7 +31807,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -31671,7 +31826,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -31690,7 +31845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -31709,7 +31864,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -31728,7 +31883,7 @@
         <v>5.6338028169014086E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -31747,7 +31902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -31766,7 +31921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -31785,8 +31940,8 @@
         <v>8.4507042253521125E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="50.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="50.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -31803,7 +31958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -31824,7 +31979,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -31845,8 +32000,8 @@
         <v>0.98591549295774639</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="138.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="138.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -31860,7 +32015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -31879,7 +32034,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -31898,7 +32053,7 @@
         <v>0.9859154929577465</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -31917,7 +32072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -31936,8 +32091,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="85.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -31954,7 +32109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -31973,7 +32128,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -31992,7 +32147,7 @@
         <v>0.39436619718309857</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -32011,7 +32166,7 @@
         <v>0.26760563380281688</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -32030,7 +32185,7 @@
         <v>0.15492957746478872</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -32049,7 +32204,7 @@
         <v>8.4507042253521125E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -32068,7 +32223,7 @@
         <v>5.6338028169014086E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -32087,7 +32242,7 @@
         <v>1.4084507042253521E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -32106,7 +32261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -32125,7 +32280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11</v>
       </c>
@@ -32144,7 +32299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12</v>
       </c>
@@ -32163,7 +32318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16</v>
       </c>
@@ -32182,7 +32337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
@@ -32201,8 +32356,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -32219,7 +32374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -32238,7 +32393,7 @@
         <v>1.3245033112582781E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -32257,7 +32412,7 @@
         <v>3.3112582781456956E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -32276,7 +32431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -32295,7 +32450,7 @@
         <v>6.6225165562913907E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -32314,7 +32469,7 @@
         <v>2.6490066225165563E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -32333,7 +32488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -32352,7 +32507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -32371,7 +32526,7 @@
         <v>2.6490066225165563E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -32390,7 +32545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -32409,7 +32564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -32428,7 +32583,7 @@
         <v>0.85430463576158944</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -32447,8 +32602,8 @@
         <v>3.9735099337748346E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="56.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -32465,7 +32620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -32484,7 +32639,7 @@
         <v>0.11267605633802817</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -32503,7 +32658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -32522,7 +32677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -32541,7 +32696,7 @@
         <v>7.0422535211267609E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -32560,7 +32715,7 @@
         <v>0.26760563380281688</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>38</v>
       </c>
@@ -32579,7 +32734,7 @@
         <v>2.8169014084507043E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>39</v>
       </c>
@@ -32598,7 +32753,7 @@
         <v>0.45070422535211269</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>40</v>
       </c>
@@ -32617,7 +32772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -32636,8 +32791,8 @@
         <v>7.0422535211267609E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="103.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="103.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>53</v>
       </c>
@@ -32654,7 +32809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -32673,7 +32828,7 @@
         <v>0.36619718309859156</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -32692,8 +32847,8 @@
         <v>0.63380281690140849</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="162" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="162" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -32710,7 +32865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -32729,7 +32884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1</v>
       </c>
@@ -32748,7 +32903,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2</v>
       </c>
@@ -32767,7 +32922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3</v>
       </c>
@@ -32786,7 +32941,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>4</v>
       </c>
@@ -32805,7 +32960,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5</v>
       </c>
@@ -32824,7 +32979,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>6</v>
       </c>
@@ -32843,7 +32998,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>7</v>
       </c>
@@ -32862,7 +33017,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8</v>
       </c>
@@ -32881,7 +33036,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9</v>
       </c>
@@ -32900,7 +33055,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>10</v>
       </c>
@@ -32919,7 +33074,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>11</v>
       </c>
@@ -32938,7 +33093,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>12</v>
       </c>
@@ -32957,7 +33112,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>13</v>
       </c>
@@ -32976,7 +33131,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>14</v>
       </c>
@@ -32995,7 +33150,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>15</v>
       </c>
@@ -33014,7 +33169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>16</v>
       </c>
@@ -33033,7 +33188,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>17</v>
       </c>
@@ -33052,7 +33207,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>18</v>
       </c>
@@ -33071,7 +33226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>19</v>
       </c>
@@ -33090,7 +33245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>20</v>
       </c>
@@ -33109,7 +33264,7 @@
         <v>5.7971014492753624E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>21</v>
       </c>
@@ -33128,7 +33283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>22</v>
       </c>
@@ -33147,7 +33302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>23</v>
       </c>
@@ -33166,7 +33321,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>24</v>
       </c>
@@ -33185,7 +33340,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>25</v>
       </c>
@@ -33204,7 +33359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>26</v>
       </c>
@@ -33223,7 +33378,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>27</v>
       </c>
@@ -33242,7 +33397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>28</v>
       </c>
@@ -33261,7 +33416,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>29</v>
       </c>
@@ -33280,7 +33435,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>30</v>
       </c>
@@ -33299,7 +33454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>31</v>
       </c>
@@ -33318,7 +33473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>32</v>
       </c>
@@ -33337,7 +33492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>33</v>
       </c>
@@ -33356,7 +33511,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>34</v>
       </c>
@@ -33375,7 +33530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>35</v>
       </c>
@@ -33394,7 +33549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>36</v>
       </c>
@@ -33413,7 +33568,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>37</v>
       </c>
@@ -33432,7 +33587,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>38</v>
       </c>
@@ -33451,7 +33606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>39</v>
       </c>
@@ -33470,7 +33625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>40</v>
       </c>
@@ -33489,7 +33644,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>42</v>
       </c>
@@ -33508,7 +33663,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>43</v>
       </c>
@@ -33527,7 +33682,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>46</v>
       </c>
@@ -33546,7 +33701,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>47</v>
       </c>
@@ -33565,7 +33720,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>48</v>
       </c>
@@ -33584,7 +33739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>49</v>
       </c>
@@ -33603,7 +33758,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>50</v>
       </c>
@@ -33622,7 +33777,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>264</v>
       </c>
@@ -33641,7 +33796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>128</v>
       </c>
@@ -33660,7 +33815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>52</v>
       </c>
@@ -33679,7 +33834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>53</v>
       </c>
@@ -33698,7 +33853,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>54</v>
       </c>
@@ -33717,7 +33872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>56</v>
       </c>
@@ -33736,7 +33891,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>57</v>
       </c>
@@ -33755,7 +33910,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>58</v>
       </c>
@@ -33774,7 +33929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>59</v>
       </c>
@@ -33793,7 +33948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>60</v>
       </c>
@@ -33812,7 +33967,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>138</v>
       </c>
@@ -33831,7 +33986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>62</v>
       </c>
@@ -33850,7 +34005,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>63</v>
       </c>
@@ -33869,7 +34024,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>65</v>
       </c>
@@ -33888,7 +34043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>67</v>
       </c>
@@ -33907,7 +34062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>68</v>
       </c>
@@ -33926,7 +34081,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>69</v>
       </c>
@@ -33945,7 +34100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>72</v>
       </c>
@@ -33964,7 +34119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>129</v>
       </c>
@@ -33983,7 +34138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>74</v>
       </c>
@@ -34002,7 +34157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>76</v>
       </c>
@@ -34021,7 +34176,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>78</v>
       </c>
@@ -34040,7 +34195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>207</v>
       </c>
@@ -34059,7 +34214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>49</v>
       </c>
@@ -34078,7 +34233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>84</v>
       </c>
@@ -34097,7 +34252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>86</v>
       </c>
@@ -34116,7 +34271,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>90</v>
       </c>
@@ -34135,7 +34290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>92</v>
       </c>
@@ -34154,7 +34309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>94</v>
       </c>
@@ -34173,7 +34328,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>956</v>
       </c>
@@ -34192,7 +34347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>110</v>
       </c>
@@ -34211,7 +34366,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>239</v>
       </c>
@@ -34230,7 +34385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>114</v>
       </c>
@@ -34249,7 +34404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>118</v>
       </c>
@@ -34268,7 +34423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>120</v>
       </c>
@@ -34287,7 +34442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>121</v>
       </c>
@@ -34306,7 +34461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>123</v>
       </c>
@@ -34325,7 +34480,7 @@
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>49</v>
       </c>
@@ -34342,7 +34497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>46</v>
       </c>
@@ -34361,7 +34516,7 @@
         <v>0.11267605633802817</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>47</v>
       </c>
@@ -34380,7 +34535,7 @@
         <v>0.88732394366197187</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>48</v>
       </c>

</xml_diff>